<commit_message>
enhance(puerto rico): add teritory
</commit_message>
<xml_diff>
--- a/public/data/testing/covid-testing-latest-data-source-details.xlsx
+++ b/public/data/testing/covid-testing-latest-data-source-details.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="925" uniqueCount="925">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="928" uniqueCount="928">
   <si>
     <t xml:space="preserve">ISO code</t>
   </si>
@@ -1518,7 +1518,7 @@
     <t xml:space="preserve">Jamaica - samples tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.moh.gov.jm/covid-19-clinical-management-summary-for-wednesday-march-23-2022/</t>
+    <t xml:space="preserve">https://www.moh.gov.jm/covid-19-clinical-management-summary-for-monday-march-28-2022/</t>
   </si>
   <si>
     <t xml:space="preserve">Jamaica Ministry of Health and Wellness</t>
@@ -2193,7 +2193,7 @@
     <t xml:space="preserve">Palestine - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.facebook.com/mohps/posts/pfbid031YuxVi7tQ7xggCWahCNEqnu31nNwB53PrBhHqSmU8C9B1t7zDRsnNWbf2Qf93pDtl?__cft__[0]=AZVh7w_qvT6FL0hwNzWUYISLrIp7ItQaxIIiMygkitGjbhLrgGOOnnxKZP_kyWVGr66586rhPzyR9qDctKuKpbRJ35WB4x4h4cLASjAzu1r6PheQ0-tgHI4GdfH-ah_4m2ju3Ej4uB87wZQr-6v5MPR_bh3YOKkW4sD6v79L0QdmAg&amp;__tn__=%2CO%2CP-R</t>
+    <t xml:space="preserve">https://web.facebook.com/mohps/posts/322661553294147</t>
   </si>
   <si>
     <t xml:space="preserve">Palestinian Ministry of Health</t>
@@ -2215,7 +2215,7 @@
     <t xml:space="preserve">Panama - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://twitter.com/MINSAPma/status/1507126839071977476</t>
+    <t xml:space="preserve">https://twitter.com/MINSAPma/status/1508968977707544578</t>
   </si>
   <si>
     <t xml:space="preserve">Panama Ministry of Health</t>
@@ -2338,6 +2338,27 @@
     <t xml:space="preserve">The dashboard provides figures for the number of samples processed, both as daily figures and as cumulative figure since 1 March 2020.
 Up until 29 April 2020 we had reported a figure of the number of people tested, obtained as the sum of confirmed and unconfirmed cases in the Portugal Ministry of Health (MOH) [daily updates](https://covid19.min-saude.pt/relatorio-de-situacao/). We were alerted by a Technical Advisor within the Cabinet of the Secretary of Health to the fact that these figures only captures people who were reported through the National System of Epidemiological Surveillance which does not include many of the people that get tested but are never entered into the surveillance system (because they do not meet the criteria and go on to test negatively). For this reason we have now switched to the current series. The advisor confirmed to us that this series: includes all the public, private and university labs performing SARS-CoV-2 diagnosis in Portugal; does not include tests pending results.
 Since October 2020, rapid antigen tests are also being performed for the diagnosis of COVID-19 in Portugal. Since positive results from these antigen tests are notified and counted in daily national figures for confirmed cases, we include them in the number of tests performed in the country. Some laboratories are performing PCR confirmatory tests on both negative and positive antigen tests.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PRI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Puerto Rico - tests performed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://healthdata.gov/dataset/COVID-19-Diagnostic-Laboratory-Testing-PCR-Testing/j8mb-icvb</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Department of Health &amp; Human Services</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The number of tests performed. The figures are the sum across states, some of which may include serology and antigen tests in addition to PCR tests.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Our principal time series for Puerto Rico is based on the CSV file made available by the Department of Health &amp; Human Services on HealthData.gov.
+According to the metadata, the data "is representative of diagnostic specimens being tested - not individual people (...). Data presented might not represent the most current counts for the most recent 3 days due to the time it takes to report testing information. The data may also not include results from all potential testing sites within the jurisdiction (e.g., non-laboratory or point of care test sites)."
+It is also explained in the description that the data "excludes serology tests where possible", which may indicate that not 100% of the tests included in the time series are PCR tests.
+Note that due to the great diversity of counting methods across US states for both cases and tests, calculating an accurate positive rate for the entire country can be very challenging. The volunteer-led COVID Tracking Project has a very useful blog post summarizing these obstacles: '[Test Positivity in the US Is a Mess](https://covidtracking.com/analysis-updates/test-positivity-in-the-us-is-a-mess)'.</t>
   </si>
   <si>
     <t xml:space="preserve">QAT</t>
@@ -2987,15 +3008,6 @@
   </si>
   <si>
     <t xml:space="preserve">United States - tests performed</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://healthdata.gov/dataset/COVID-19-Diagnostic-Laboratory-Testing-PCR-Testing/j8mb-icvb</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Department of Health &amp; Human Services</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The number of tests performed. The figures are the sum across states, some of which may include serology tests in addition to PCR tests.</t>
   </si>
   <si>
     <t xml:space="preserve">Since August 2020, our principal time series for the United States is based on the CSV file made available by the Department of Health &amp; Human Services on HealthData.gov.
@@ -3741,8 +3753,12 @@
       <c r="M6" t="n">
         <v>0.053</v>
       </c>
-      <c r="N6"/>
-      <c r="O6"/>
+      <c r="N6" t="n">
+        <v>0.0083</v>
+      </c>
+      <c r="O6" t="n">
+        <v>120</v>
+      </c>
       <c r="P6" t="s">
         <v>36</v>
       </c>
@@ -3963,8 +3979,12 @@
       <c r="M10" t="n">
         <v>4.219</v>
       </c>
-      <c r="N10"/>
-      <c r="O10"/>
+      <c r="N10" t="n">
+        <v>0.5062</v>
+      </c>
+      <c r="O10" t="n">
+        <v>2</v>
+      </c>
       <c r="P10" t="s">
         <v>71</v>
       </c>
@@ -4016,8 +4036,12 @@
       <c r="M11" t="n">
         <v>46.592</v>
       </c>
-      <c r="N11"/>
-      <c r="O11"/>
+      <c r="N11" t="n">
+        <v>0.0846</v>
+      </c>
+      <c r="O11" t="n">
+        <v>11.8</v>
+      </c>
       <c r="P11" t="s">
         <v>78</v>
       </c>
@@ -4065,8 +4089,12 @@
       <c r="M12" t="n">
         <v>0.237</v>
       </c>
-      <c r="N12"/>
-      <c r="O12"/>
+      <c r="N12" t="n">
+        <v>0.015</v>
+      </c>
+      <c r="O12" t="n">
+        <v>66.6</v>
+      </c>
       <c r="P12" t="s">
         <v>83</v>
       </c>
@@ -4167,8 +4195,12 @@
       <c r="M14" t="n">
         <v>3.271</v>
       </c>
-      <c r="N14"/>
-      <c r="O14"/>
+      <c r="N14" t="n">
+        <v>0.1597</v>
+      </c>
+      <c r="O14" t="n">
+        <v>6.3</v>
+      </c>
       <c r="P14" t="s">
         <v>95</v>
       </c>
@@ -4220,8 +4252,12 @@
       <c r="M15" t="n">
         <v>0.018</v>
       </c>
-      <c r="N15"/>
-      <c r="O15"/>
+      <c r="N15" t="n">
+        <v>0.0297</v>
+      </c>
+      <c r="O15" t="n">
+        <v>33.7</v>
+      </c>
       <c r="P15" t="s">
         <v>102</v>
       </c>
@@ -4322,8 +4358,12 @@
       <c r="M17" t="n">
         <v>1.275</v>
       </c>
-      <c r="N17"/>
-      <c r="O17"/>
+      <c r="N17" t="n">
+        <v>0.0955</v>
+      </c>
+      <c r="O17" t="n">
+        <v>10.5</v>
+      </c>
       <c r="P17" t="s">
         <v>113</v>
       </c>
@@ -4901,8 +4941,12 @@
       <c r="M28" t="n">
         <v>0.179</v>
       </c>
-      <c r="N28"/>
-      <c r="O28"/>
+      <c r="N28" t="n">
+        <v>0.0059</v>
+      </c>
+      <c r="O28" t="n">
+        <v>168.8</v>
+      </c>
       <c r="P28" t="s">
         <v>36</v>
       </c>
@@ -4950,8 +4994,12 @@
       <c r="M29" t="n">
         <v>0.072</v>
       </c>
-      <c r="N29"/>
-      <c r="O29"/>
+      <c r="N29" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="O29" t="n">
+        <v>20</v>
+      </c>
       <c r="P29" t="s">
         <v>176</v>
       </c>
@@ -5262,8 +5310,12 @@
       <c r="M35" t="n">
         <v>4.033</v>
       </c>
-      <c r="N35"/>
-      <c r="O35"/>
+      <c r="N35" t="n">
+        <v>0.0994</v>
+      </c>
+      <c r="O35" t="n">
+        <v>10.1</v>
+      </c>
       <c r="P35" t="s">
         <v>202</v>
       </c>
@@ -5523,8 +5575,12 @@
       <c r="M40" t="n">
         <v>0.055</v>
       </c>
-      <c r="N40"/>
-      <c r="O40"/>
+      <c r="N40" t="n">
+        <v>0.0045</v>
+      </c>
+      <c r="O40" t="n">
+        <v>223.4</v>
+      </c>
       <c r="P40" t="s">
         <v>36</v>
       </c>
@@ -5572,8 +5628,12 @@
       <c r="M41" t="n">
         <v>1.27</v>
       </c>
-      <c r="N41"/>
-      <c r="O41"/>
+      <c r="N41" t="n">
+        <v>0.2728</v>
+      </c>
+      <c r="O41" t="n">
+        <v>3.7</v>
+      </c>
       <c r="P41" t="s">
         <v>231</v>
       </c>
@@ -5904,8 +5964,12 @@
       <c r="M47" t="n">
         <v>0.414</v>
       </c>
-      <c r="N47"/>
-      <c r="O47"/>
+      <c r="N47" t="n">
+        <v>0.0041</v>
+      </c>
+      <c r="O47" t="n">
+        <v>242.1</v>
+      </c>
       <c r="P47" t="s">
         <v>36</v>
       </c>
@@ -6069,8 +6133,12 @@
       <c r="M50" t="n">
         <v>0.01</v>
       </c>
-      <c r="N50"/>
-      <c r="O50"/>
+      <c r="N50" t="n">
+        <v>0.7733</v>
+      </c>
+      <c r="O50" t="n">
+        <v>1.3</v>
+      </c>
       <c r="P50" t="s">
         <v>36</v>
       </c>
@@ -6330,8 +6398,12 @@
       <c r="M55" t="n">
         <v>0.917</v>
       </c>
-      <c r="N55"/>
-      <c r="O55"/>
+      <c r="N55" t="n">
+        <v>0.0145</v>
+      </c>
+      <c r="O55" t="n">
+        <v>69</v>
+      </c>
       <c r="P55" t="s">
         <v>36</v>
       </c>
@@ -6379,8 +6451,12 @@
       <c r="M56" t="n">
         <v>0.042</v>
       </c>
-      <c r="N56"/>
-      <c r="O56"/>
+      <c r="N56" t="n">
+        <v>0.0055</v>
+      </c>
+      <c r="O56" t="n">
+        <v>183.4</v>
+      </c>
       <c r="P56" t="s">
         <v>303</v>
       </c>
@@ -6860,8 +6936,12 @@
       <c r="M65" t="n">
         <v>0.098</v>
       </c>
-      <c r="N65"/>
-      <c r="O65"/>
+      <c r="N65" t="n">
+        <v>0.0028</v>
+      </c>
+      <c r="O65" t="n">
+        <v>352.2</v>
+      </c>
       <c r="P65" t="s">
         <v>36</v>
       </c>
@@ -6909,8 +6989,12 @@
       <c r="M66" t="n">
         <v>15.464</v>
       </c>
-      <c r="N66"/>
-      <c r="O66"/>
+      <c r="N66" t="n">
+        <v>0.1481</v>
+      </c>
+      <c r="O66" t="n">
+        <v>6.8</v>
+      </c>
       <c r="P66" t="s">
         <v>358</v>
       </c>
@@ -6958,8 +7042,12 @@
       <c r="M67" t="n">
         <v>24.842</v>
       </c>
-      <c r="N67"/>
-      <c r="O67"/>
+      <c r="N67" t="n">
+        <v>0.0808</v>
+      </c>
+      <c r="O67" t="n">
+        <v>12.4</v>
+      </c>
       <c r="P67" t="s">
         <v>364</v>
       </c>
@@ -7117,8 +7205,12 @@
       <c r="M70" t="n">
         <v>0.069</v>
       </c>
-      <c r="N70"/>
-      <c r="O70"/>
+      <c r="N70" t="n">
+        <v>0.0276</v>
+      </c>
+      <c r="O70" t="n">
+        <v>36.3</v>
+      </c>
       <c r="P70" t="s">
         <v>36</v>
       </c>
@@ -7331,8 +7423,12 @@
       <c r="M74" t="n">
         <v>1.01</v>
       </c>
-      <c r="N74"/>
-      <c r="O74"/>
+      <c r="N74" t="n">
+        <v>0.2152</v>
+      </c>
+      <c r="O74" t="n">
+        <v>4.6</v>
+      </c>
       <c r="P74" t="s">
         <v>403</v>
       </c>
@@ -7549,8 +7645,12 @@
       <c r="M78" t="n">
         <v>0.734</v>
       </c>
-      <c r="N78"/>
-      <c r="O78"/>
+      <c r="N78" t="n">
+        <v>0.0268</v>
+      </c>
+      <c r="O78" t="n">
+        <v>37.3</v>
+      </c>
       <c r="P78" t="s">
         <v>428</v>
       </c>
@@ -7655,8 +7755,12 @@
       <c r="M80" t="n">
         <v>3.437</v>
       </c>
-      <c r="N80"/>
-      <c r="O80"/>
+      <c r="N80" t="n">
+        <v>0.4397</v>
+      </c>
+      <c r="O80" t="n">
+        <v>2.3</v>
+      </c>
       <c r="P80" t="s">
         <v>436</v>
       </c>
@@ -7767,8 +7871,12 @@
       <c r="M82" t="n">
         <v>7.821</v>
       </c>
-      <c r="N82"/>
-      <c r="O82"/>
+      <c r="N82" t="n">
+        <v>0.1516</v>
+      </c>
+      <c r="O82" t="n">
+        <v>6.6</v>
+      </c>
       <c r="P82" t="s">
         <v>450</v>
       </c>
@@ -7790,7 +7898,7 @@
         <v>454</v>
       </c>
       <c r="C83" s="1" t="n">
-        <v>44643</v>
+        <v>44648</v>
       </c>
       <c r="D83" t="s">
         <v>455</v>
@@ -7800,31 +7908,31 @@
       </c>
       <c r="F83"/>
       <c r="G83" t="n">
-        <v>523</v>
+        <v>528</v>
       </c>
       <c r="H83" t="n">
-        <v>907881</v>
+        <v>922458</v>
       </c>
       <c r="I83" t="n">
-        <v>305.328</v>
+        <v>310.23</v>
       </c>
       <c r="J83" t="n">
-        <v>2309</v>
+        <v>2310</v>
       </c>
       <c r="K83" t="n">
         <v>0.777</v>
       </c>
       <c r="L83" t="n">
-        <v>2561</v>
+        <v>2712</v>
       </c>
       <c r="M83" t="n">
-        <v>0.861</v>
+        <v>0.912</v>
       </c>
       <c r="N83" t="n">
-        <v>0.0094</v>
+        <v>0.0073</v>
       </c>
       <c r="O83" t="n">
-        <v>106.7</v>
+        <v>136.6</v>
       </c>
       <c r="P83" t="s">
         <v>456</v>
@@ -8040,8 +8148,12 @@
       <c r="M87" t="n">
         <v>0.067</v>
       </c>
-      <c r="N87"/>
-      <c r="O87"/>
+      <c r="N87" t="n">
+        <v>0.0037</v>
+      </c>
+      <c r="O87" t="n">
+        <v>272.3</v>
+      </c>
       <c r="P87" t="s">
         <v>36</v>
       </c>
@@ -8254,8 +8366,12 @@
       <c r="M91" t="n">
         <v>4.027</v>
       </c>
-      <c r="N91"/>
-      <c r="O91"/>
+      <c r="N91" t="n">
+        <v>0.364</v>
+      </c>
+      <c r="O91" t="n">
+        <v>2.7</v>
+      </c>
       <c r="P91" t="s">
         <v>500</v>
       </c>
@@ -8352,8 +8468,12 @@
       <c r="M93" t="n">
         <v>0.563</v>
       </c>
-      <c r="N93"/>
-      <c r="O93"/>
+      <c r="N93" t="n">
+        <v>0.0123</v>
+      </c>
+      <c r="O93" t="n">
+        <v>81.1</v>
+      </c>
       <c r="P93" t="s">
         <v>36</v>
       </c>
@@ -8715,8 +8835,12 @@
       <c r="M100" t="n">
         <v>0.021</v>
       </c>
-      <c r="N100"/>
-      <c r="O100"/>
+      <c r="N100" t="n">
+        <v>0.0197</v>
+      </c>
+      <c r="O100" t="n">
+        <v>50.8</v>
+      </c>
       <c r="P100" t="s">
         <v>36</v>
       </c>
@@ -8880,8 +9004,12 @@
       <c r="M103" t="n">
         <v>0.047</v>
       </c>
-      <c r="N103"/>
-      <c r="O103"/>
+      <c r="N103" t="n">
+        <v>0.0028</v>
+      </c>
+      <c r="O103" t="n">
+        <v>358.9</v>
+      </c>
       <c r="P103" t="s">
         <v>36</v>
       </c>
@@ -9182,8 +9310,12 @@
       <c r="M109" t="n">
         <v>1.057</v>
       </c>
-      <c r="N109"/>
-      <c r="O109"/>
+      <c r="N109" t="n">
+        <v>0.0671</v>
+      </c>
+      <c r="O109" t="n">
+        <v>14.9</v>
+      </c>
       <c r="P109" t="s">
         <v>53</v>
       </c>
@@ -9231,8 +9363,12 @@
       <c r="M110" t="n">
         <v>0.179</v>
       </c>
-      <c r="N110"/>
-      <c r="O110"/>
+      <c r="N110" t="n">
+        <v>0.0101</v>
+      </c>
+      <c r="O110" t="n">
+        <v>98.8</v>
+      </c>
       <c r="P110" t="s">
         <v>594</v>
       </c>
@@ -9280,8 +9416,12 @@
       <c r="M111" t="n">
         <v>0.021</v>
       </c>
-      <c r="N111"/>
-      <c r="O111"/>
+      <c r="N111" t="n">
+        <v>0.006</v>
+      </c>
+      <c r="O111" t="n">
+        <v>167.8</v>
+      </c>
       <c r="P111" t="s">
         <v>36</v>
       </c>
@@ -9382,8 +9522,12 @@
       <c r="M113" t="n">
         <v>0.323</v>
       </c>
-      <c r="N113"/>
-      <c r="O113"/>
+      <c r="N113" t="n">
+        <v>0.0157</v>
+      </c>
+      <c r="O113" t="n">
+        <v>63.7</v>
+      </c>
       <c r="P113" t="s">
         <v>608</v>
       </c>
@@ -9590,8 +9734,12 @@
       <c r="M117" t="n">
         <v>0.019</v>
       </c>
-      <c r="N117"/>
-      <c r="O117"/>
+      <c r="N117" t="n">
+        <v>0.0021</v>
+      </c>
+      <c r="O117" t="n">
+        <v>474</v>
+      </c>
       <c r="P117" t="s">
         <v>36</v>
       </c>
@@ -9692,8 +9840,12 @@
       <c r="M119" t="n">
         <v>1.106</v>
       </c>
-      <c r="N119"/>
-      <c r="O119"/>
+      <c r="N119" t="n">
+        <v>0.1052</v>
+      </c>
+      <c r="O119" t="n">
+        <v>9.5</v>
+      </c>
       <c r="P119" t="s">
         <v>53</v>
       </c>
@@ -9847,8 +9999,12 @@
       <c r="M122" t="n">
         <v>0.135</v>
       </c>
-      <c r="N122"/>
-      <c r="O122"/>
+      <c r="N122" t="n">
+        <v>0.0091</v>
+      </c>
+      <c r="O122" t="n">
+        <v>109.8</v>
+      </c>
       <c r="P122" t="s">
         <v>652</v>
       </c>
@@ -9870,7 +10026,7 @@
         <v>655</v>
       </c>
       <c r="C123" s="1" t="n">
-        <v>44643</v>
+        <v>44647</v>
       </c>
       <c r="D123" t="s">
         <v>656</v>
@@ -9880,15 +10036,15 @@
       </c>
       <c r="F123"/>
       <c r="G123" t="n">
-        <v>553</v>
+        <v>554</v>
       </c>
       <c r="H123"/>
       <c r="I123"/>
       <c r="J123" t="n">
-        <v>4471</v>
+        <v>3815</v>
       </c>
       <c r="K123" t="n">
-        <v>0.856</v>
+        <v>0.73</v>
       </c>
       <c r="L123"/>
       <c r="M123"/>
@@ -9915,7 +10071,7 @@
         <v>661</v>
       </c>
       <c r="C124" s="1" t="n">
-        <v>44644</v>
+        <v>44649</v>
       </c>
       <c r="D124" t="s">
         <v>662</v>
@@ -9925,27 +10081,31 @@
       </c>
       <c r="F124"/>
       <c r="G124" t="n">
-        <v>728</v>
+        <v>733</v>
       </c>
       <c r="H124" t="n">
-        <v>5656308</v>
+        <v>5686445</v>
       </c>
       <c r="I124" t="n">
-        <v>1290.928</v>
-      </c>
-      <c r="J124"/>
-      <c r="K124"/>
+        <v>1297.806</v>
+      </c>
+      <c r="J124" t="n">
+        <v>7696</v>
+      </c>
+      <c r="K124" t="n">
+        <v>1.756</v>
+      </c>
       <c r="L124" t="n">
-        <v>6206</v>
+        <v>6322</v>
       </c>
       <c r="M124" t="n">
-        <v>1.416</v>
+        <v>1.443</v>
       </c>
       <c r="N124" t="n">
-        <v>0.046</v>
+        <v>0.0435</v>
       </c>
       <c r="O124" t="n">
-        <v>21.7</v>
+        <v>23</v>
       </c>
       <c r="P124" t="s">
         <v>663</v>
@@ -10284,7 +10444,7 @@
         <v>701</v>
       </c>
       <c r="C131" s="1" t="n">
-        <v>44647</v>
+        <v>44646</v>
       </c>
       <c r="D131" t="s">
         <v>702</v>
@@ -10294,139 +10454,139 @@
       </c>
       <c r="F131"/>
       <c r="G131" t="n">
-        <v>281</v>
+        <v>755</v>
       </c>
       <c r="H131" t="n">
-        <v>6333416</v>
+        <v>2622514</v>
       </c>
       <c r="I131" t="n">
-        <v>2161.189</v>
+        <v>927.258</v>
       </c>
       <c r="J131" t="n">
-        <v>21316</v>
+        <v>998</v>
       </c>
       <c r="K131" t="n">
-        <v>7.274</v>
+        <v>0.353</v>
       </c>
       <c r="L131" t="n">
-        <v>19035</v>
+        <v>1866</v>
       </c>
       <c r="M131" t="n">
-        <v>6.495</v>
+        <v>0.66</v>
       </c>
       <c r="N131"/>
       <c r="O131"/>
       <c r="P131" t="s">
+        <v>703</v>
+      </c>
+      <c r="Q131" t="s">
+        <v>702</v>
+      </c>
+      <c r="R131" t="s">
         <v>704</v>
       </c>
-      <c r="Q131" t="s">
+      <c r="S131" t="s">
         <v>705</v>
-      </c>
-      <c r="R131" t="s">
-        <v>45</v>
-      </c>
-      <c r="S131" t="s">
-        <v>706</v>
       </c>
     </row>
     <row r="132">
       <c r="A132" t="s">
+        <v>706</v>
+      </c>
+      <c r="B132" t="s">
         <v>707</v>
       </c>
-      <c r="B132" t="s">
+      <c r="C132" s="1" t="n">
+        <v>44647</v>
+      </c>
+      <c r="D132" t="s">
         <v>708</v>
       </c>
-      <c r="C132" s="1" t="n">
-        <v>44630</v>
-      </c>
-      <c r="D132" t="s">
-        <v>691</v>
-      </c>
       <c r="E132" t="s">
-        <v>692</v>
+        <v>709</v>
       </c>
       <c r="F132"/>
       <c r="G132" t="n">
-        <v>104</v>
+        <v>281</v>
       </c>
       <c r="H132" t="n">
-        <v>21260367</v>
+        <v>6333416</v>
       </c>
       <c r="I132" t="n">
-        <v>1111.492</v>
-      </c>
-      <c r="J132"/>
-      <c r="K132"/>
+        <v>2161.189</v>
+      </c>
+      <c r="J132" t="n">
+        <v>21316</v>
+      </c>
+      <c r="K132" t="n">
+        <v>7.274</v>
+      </c>
       <c r="L132" t="n">
-        <v>75700</v>
+        <v>19035</v>
       </c>
       <c r="M132" t="n">
-        <v>3.958</v>
-      </c>
-      <c r="N132" t="n">
-        <v>0.0565</v>
-      </c>
-      <c r="O132" t="n">
-        <v>17.7</v>
-      </c>
+        <v>6.495</v>
+      </c>
+      <c r="N132"/>
+      <c r="O132"/>
       <c r="P132" t="s">
-        <v>693</v>
+        <v>710</v>
       </c>
       <c r="Q132" t="s">
-        <v>691</v>
+        <v>711</v>
       </c>
       <c r="R132" t="s">
-        <v>61</v>
+        <v>45</v>
       </c>
       <c r="S132" t="s">
-        <v>709</v>
+        <v>712</v>
       </c>
     </row>
     <row r="133">
       <c r="A133" t="s">
-        <v>710</v>
+        <v>713</v>
       </c>
       <c r="B133" t="s">
-        <v>711</v>
+        <v>714</v>
       </c>
       <c r="C133" s="1" t="n">
-        <v>44647</v>
+        <v>44630</v>
       </c>
       <c r="D133" t="s">
-        <v>712</v>
+        <v>691</v>
       </c>
       <c r="E133" t="s">
-        <v>713</v>
+        <v>692</v>
       </c>
       <c r="F133"/>
       <c r="G133" t="n">
-        <v>562</v>
+        <v>104</v>
       </c>
       <c r="H133" t="n">
-        <v>283967438</v>
+        <v>21260367</v>
       </c>
       <c r="I133" t="n">
-        <v>1946.155</v>
+        <v>1111.492</v>
       </c>
       <c r="J133"/>
       <c r="K133"/>
       <c r="L133" t="n">
-        <v>233860</v>
+        <v>75700</v>
       </c>
       <c r="M133" t="n">
-        <v>1.603</v>
+        <v>3.958</v>
       </c>
       <c r="N133" t="n">
-        <v>0.108</v>
+        <v>0.0565</v>
       </c>
       <c r="O133" t="n">
-        <v>9.3</v>
+        <v>17.7</v>
       </c>
       <c r="P133" t="s">
-        <v>713</v>
+        <v>693</v>
       </c>
       <c r="Q133" t="s">
-        <v>714</v>
+        <v>691</v>
       </c>
       <c r="R133" t="s">
         <v>61</v>
@@ -10443,7 +10603,7 @@
         <v>717</v>
       </c>
       <c r="C134" s="1" t="n">
-        <v>44648</v>
+        <v>44647</v>
       </c>
       <c r="D134" t="s">
         <v>718</v>
@@ -10453,28 +10613,28 @@
       </c>
       <c r="F134"/>
       <c r="G134" t="n">
-        <v>598</v>
+        <v>562</v>
       </c>
       <c r="H134" t="n">
-        <v>5081757</v>
+        <v>283967438</v>
       </c>
       <c r="I134" t="n">
-        <v>382.763</v>
-      </c>
-      <c r="J134" t="n">
-        <v>7798</v>
-      </c>
-      <c r="K134" t="n">
-        <v>0.587</v>
-      </c>
+        <v>1946.155</v>
+      </c>
+      <c r="J134"/>
+      <c r="K134"/>
       <c r="L134" t="n">
-        <v>8209</v>
+        <v>233860</v>
       </c>
       <c r="M134" t="n">
-        <v>0.618</v>
-      </c>
-      <c r="N134"/>
-      <c r="O134"/>
+        <v>1.603</v>
+      </c>
+      <c r="N134" t="n">
+        <v>0.108</v>
+      </c>
+      <c r="O134" t="n">
+        <v>9.3</v>
+      </c>
       <c r="P134" t="s">
         <v>719</v>
       </c>
@@ -10482,7 +10642,7 @@
         <v>720</v>
       </c>
       <c r="R134" t="s">
-        <v>136</v>
+        <v>61</v>
       </c>
       <c r="S134" t="s">
         <v>721</v>
@@ -10502,303 +10662,317 @@
         <v>724</v>
       </c>
       <c r="E135" t="s">
-        <v>53</v>
+        <v>725</v>
       </c>
       <c r="F135"/>
       <c r="G135" t="n">
-        <v>134</v>
+        <v>598</v>
       </c>
       <c r="H135" t="n">
-        <v>67821</v>
+        <v>5081757</v>
       </c>
       <c r="I135" t="n">
-        <v>1266.593</v>
-      </c>
-      <c r="J135"/>
-      <c r="K135"/>
+        <v>382.763</v>
+      </c>
+      <c r="J135" t="n">
+        <v>7798</v>
+      </c>
+      <c r="K135" t="n">
+        <v>0.587</v>
+      </c>
       <c r="L135" t="n">
-        <v>44</v>
+        <v>8209</v>
       </c>
       <c r="M135" t="n">
-        <v>0.822</v>
-      </c>
-      <c r="N135"/>
-      <c r="O135"/>
+        <v>0.618</v>
+      </c>
+      <c r="N135" t="n">
+        <v>0.0009</v>
+      </c>
+      <c r="O135" t="n">
+        <v>1064.2</v>
+      </c>
       <c r="P135" t="s">
-        <v>53</v>
+        <v>725</v>
       </c>
       <c r="Q135" t="s">
-        <v>725</v>
+        <v>726</v>
       </c>
       <c r="R135" t="s">
-        <v>311</v>
+        <v>136</v>
       </c>
       <c r="S135" t="s">
-        <v>726</v>
+        <v>727</v>
       </c>
     </row>
     <row r="136">
       <c r="A136" t="s">
-        <v>727</v>
+        <v>728</v>
       </c>
       <c r="B136" t="s">
-        <v>728</v>
+        <v>729</v>
       </c>
       <c r="C136" s="1" t="n">
         <v>44648</v>
       </c>
       <c r="D136" t="s">
-        <v>729</v>
+        <v>730</v>
       </c>
       <c r="E136" t="s">
-        <v>88</v>
+        <v>53</v>
       </c>
       <c r="F136"/>
       <c r="G136" t="n">
-        <v>15</v>
+        <v>134</v>
       </c>
       <c r="H136" t="n">
-        <v>140271</v>
+        <v>67821</v>
       </c>
       <c r="I136" t="n">
-        <v>760.685</v>
+        <v>1266.593</v>
       </c>
       <c r="J136"/>
       <c r="K136"/>
       <c r="L136" t="n">
-        <v>141</v>
+        <v>44</v>
       </c>
       <c r="M136" t="n">
-        <v>0.765</v>
-      </c>
-      <c r="N136"/>
-      <c r="O136"/>
+        <v>0.822</v>
+      </c>
+      <c r="N136" t="n">
+        <v>0.0032</v>
+      </c>
+      <c r="O136" t="n">
+        <v>307.7</v>
+      </c>
       <c r="P136" t="s">
-        <v>88</v>
+        <v>53</v>
       </c>
       <c r="Q136" t="s">
-        <v>729</v>
+        <v>731</v>
       </c>
       <c r="R136" t="s">
-        <v>25</v>
+        <v>311</v>
       </c>
       <c r="S136" t="s">
-        <v>730</v>
+        <v>732</v>
       </c>
     </row>
     <row r="137">
       <c r="A137" t="s">
-        <v>731</v>
+        <v>733</v>
       </c>
       <c r="B137" t="s">
-        <v>732</v>
+        <v>734</v>
       </c>
       <c r="C137" s="1" t="n">
-        <v>44643</v>
+        <v>44648</v>
       </c>
       <c r="D137" t="s">
-        <v>733</v>
+        <v>735</v>
       </c>
       <c r="E137" t="s">
-        <v>734</v>
+        <v>88</v>
       </c>
       <c r="F137"/>
       <c r="G137" t="n">
-        <v>61</v>
+        <v>15</v>
       </c>
       <c r="H137" t="n">
-        <v>104040</v>
+        <v>140271</v>
       </c>
       <c r="I137" t="n">
-        <v>935.031</v>
+        <v>760.685</v>
       </c>
       <c r="J137"/>
       <c r="K137"/>
       <c r="L137" t="n">
-        <v>61</v>
+        <v>141</v>
       </c>
       <c r="M137" t="n">
-        <v>0.548</v>
+        <v>0.765</v>
       </c>
       <c r="N137" t="n">
-        <v>0.0094</v>
+        <v>0.0507</v>
       </c>
       <c r="O137" t="n">
-        <v>106.8</v>
+        <v>19.7</v>
       </c>
       <c r="P137" t="s">
+        <v>88</v>
+      </c>
+      <c r="Q137" t="s">
         <v>735</v>
-      </c>
-      <c r="Q137" t="s">
-        <v>736</v>
       </c>
       <c r="R137" t="s">
         <v>25</v>
       </c>
       <c r="S137" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
     </row>
     <row r="138">
       <c r="A138" t="s">
+        <v>737</v>
+      </c>
+      <c r="B138" t="s">
         <v>738</v>
       </c>
-      <c r="B138" t="s">
+      <c r="C138" s="1" t="n">
+        <v>44643</v>
+      </c>
+      <c r="D138" t="s">
         <v>739</v>
       </c>
-      <c r="C138" s="1" t="n">
-        <v>44647</v>
-      </c>
-      <c r="D138" t="s">
+      <c r="E138" t="s">
         <v>740</v>
-      </c>
-      <c r="E138" t="s">
-        <v>53</v>
       </c>
       <c r="F138"/>
       <c r="G138" t="n">
-        <v>756</v>
+        <v>61</v>
       </c>
       <c r="H138" t="n">
-        <v>41492799</v>
+        <v>104040</v>
       </c>
       <c r="I138" t="n">
-        <v>1174.08</v>
-      </c>
-      <c r="J138" t="n">
-        <v>16463</v>
-      </c>
-      <c r="K138" t="n">
-        <v>0.466</v>
-      </c>
+        <v>935.031</v>
+      </c>
+      <c r="J138"/>
+      <c r="K138"/>
       <c r="L138" t="n">
-        <v>15063</v>
+        <v>61</v>
       </c>
       <c r="M138" t="n">
-        <v>0.426</v>
+        <v>0.548</v>
       </c>
       <c r="N138" t="n">
-        <v>0.0072</v>
+        <v>0.0094</v>
       </c>
       <c r="O138" t="n">
-        <v>138.9</v>
+        <v>106.8</v>
       </c>
       <c r="P138" t="s">
-        <v>53</v>
+        <v>741</v>
       </c>
       <c r="Q138" t="s">
-        <v>740</v>
+        <v>742</v>
       </c>
       <c r="R138" t="s">
-        <v>61</v>
+        <v>25</v>
       </c>
       <c r="S138" t="s">
-        <v>741</v>
+        <v>743</v>
       </c>
     </row>
     <row r="139">
       <c r="A139" t="s">
-        <v>742</v>
+        <v>744</v>
       </c>
       <c r="B139" t="s">
-        <v>743</v>
+        <v>745</v>
       </c>
       <c r="C139" s="1" t="n">
-        <v>44648</v>
+        <v>44647</v>
       </c>
       <c r="D139" t="s">
-        <v>744</v>
+        <v>746</v>
       </c>
       <c r="E139" t="s">
-        <v>745</v>
+        <v>53</v>
       </c>
       <c r="F139"/>
       <c r="G139" t="n">
         <v>756</v>
       </c>
       <c r="H139" t="n">
-        <v>1068046</v>
+        <v>41492799</v>
       </c>
       <c r="I139" t="n">
-        <v>62.109</v>
+        <v>1174.08</v>
       </c>
       <c r="J139" t="n">
-        <v>1246</v>
+        <v>16463</v>
       </c>
       <c r="K139" t="n">
-        <v>0.072</v>
+        <v>0.466</v>
       </c>
       <c r="L139" t="n">
-        <v>1251</v>
+        <v>15063</v>
       </c>
       <c r="M139" t="n">
-        <v>0.073</v>
-      </c>
-      <c r="N139"/>
-      <c r="O139"/>
+        <v>0.426</v>
+      </c>
+      <c r="N139" t="n">
+        <v>0.0072</v>
+      </c>
+      <c r="O139" t="n">
+        <v>138.9</v>
+      </c>
       <c r="P139" t="s">
-        <v>745</v>
+        <v>53</v>
       </c>
       <c r="Q139" t="s">
-        <v>744</v>
+        <v>746</v>
       </c>
       <c r="R139" t="s">
         <v>61</v>
       </c>
       <c r="S139" t="s">
-        <v>746</v>
+        <v>747</v>
       </c>
     </row>
     <row r="140">
       <c r="A140" t="s">
-        <v>747</v>
+        <v>748</v>
       </c>
       <c r="B140" t="s">
-        <v>748</v>
+        <v>749</v>
       </c>
       <c r="C140" s="1" t="n">
         <v>44648</v>
       </c>
       <c r="D140" t="s">
-        <v>749</v>
+        <v>750</v>
       </c>
       <c r="E140" t="s">
-        <v>53</v>
-      </c>
-      <c r="F140" t="s">
+        <v>751</v>
+      </c>
+      <c r="F140"/>
+      <c r="G140" t="n">
+        <v>756</v>
+      </c>
+      <c r="H140" t="n">
+        <v>1068046</v>
+      </c>
+      <c r="I140" t="n">
+        <v>62.109</v>
+      </c>
+      <c r="J140" t="n">
+        <v>1246</v>
+      </c>
+      <c r="K140" t="n">
+        <v>0.072</v>
+      </c>
+      <c r="L140" t="n">
+        <v>1251</v>
+      </c>
+      <c r="M140" t="n">
+        <v>0.073</v>
+      </c>
+      <c r="N140" t="n">
+        <v>0.0051</v>
+      </c>
+      <c r="O140" t="n">
+        <v>194.6</v>
+      </c>
+      <c r="P140" t="s">
+        <v>751</v>
+      </c>
+      <c r="Q140" t="s">
         <v>750</v>
       </c>
-      <c r="G140" t="n">
-        <v>761</v>
-      </c>
-      <c r="H140" t="n">
-        <v>9142320</v>
-      </c>
-      <c r="I140" t="n">
-        <v>1330.46</v>
-      </c>
-      <c r="J140" t="n">
-        <v>14076</v>
-      </c>
-      <c r="K140" t="n">
-        <v>2.048</v>
-      </c>
-      <c r="L140" t="n">
-        <v>14284</v>
-      </c>
-      <c r="M140" t="n">
-        <v>2.079</v>
-      </c>
-      <c r="N140"/>
-      <c r="O140"/>
-      <c r="P140" t="s">
-        <v>53</v>
-      </c>
-      <c r="Q140" t="s">
-        <v>751</v>
-      </c>
       <c r="R140" t="s">
-        <v>45</v>
+        <v>61</v>
       </c>
       <c r="S140" t="s">
         <v>752</v>
@@ -10812,99 +10986,105 @@
         <v>754</v>
       </c>
       <c r="C141" s="1" t="n">
-        <v>44640</v>
+        <v>44648</v>
       </c>
       <c r="D141" t="s">
-        <v>35</v>
+        <v>755</v>
       </c>
       <c r="E141" t="s">
-        <v>36</v>
-      </c>
-      <c r="F141"/>
+        <v>53</v>
+      </c>
+      <c r="F141" t="s">
+        <v>756</v>
+      </c>
       <c r="G141" t="n">
-        <v>2</v>
+        <v>761</v>
       </c>
       <c r="H141" t="n">
-        <v>390698</v>
+        <v>9142320</v>
       </c>
       <c r="I141" t="n">
-        <v>47.989</v>
-      </c>
-      <c r="J141"/>
-      <c r="K141"/>
+        <v>1330.46</v>
+      </c>
+      <c r="J141" t="n">
+        <v>14076</v>
+      </c>
+      <c r="K141" t="n">
+        <v>2.048</v>
+      </c>
       <c r="L141" t="n">
-        <v>710</v>
+        <v>14284</v>
       </c>
       <c r="M141" t="n">
-        <v>0.087</v>
+        <v>2.079</v>
       </c>
       <c r="N141" t="n">
-        <v>0.0014</v>
+        <v>0.1338</v>
       </c>
       <c r="O141" t="n">
-        <v>710</v>
+        <v>7.5</v>
       </c>
       <c r="P141" t="s">
-        <v>36</v>
+        <v>53</v>
       </c>
       <c r="Q141" t="s">
-        <v>37</v>
+        <v>757</v>
       </c>
       <c r="R141" t="s">
-        <v>25</v>
+        <v>45</v>
       </c>
       <c r="S141" t="s">
-        <v>755</v>
+        <v>758</v>
       </c>
     </row>
     <row r="142">
       <c r="A142" t="s">
-        <v>756</v>
+        <v>759</v>
       </c>
       <c r="B142" t="s">
-        <v>757</v>
+        <v>760</v>
       </c>
       <c r="C142" s="1" t="n">
-        <v>44641</v>
+        <v>44640</v>
       </c>
       <c r="D142" t="s">
-        <v>758</v>
+        <v>35</v>
       </c>
       <c r="E142" t="s">
-        <v>759</v>
+        <v>36</v>
       </c>
       <c r="F142"/>
       <c r="G142" t="n">
-        <v>70</v>
-      </c>
-      <c r="H142"/>
-      <c r="I142"/>
-      <c r="J142" t="n">
-        <v>89400</v>
-      </c>
-      <c r="K142" t="n">
-        <v>16.393</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="H142" t="n">
+        <v>390698</v>
+      </c>
+      <c r="I142" t="n">
+        <v>47.989</v>
+      </c>
+      <c r="J142"/>
+      <c r="K142"/>
       <c r="L142" t="n">
-        <v>89400</v>
+        <v>710</v>
       </c>
       <c r="M142" t="n">
-        <v>16.393</v>
+        <v>0.087</v>
       </c>
       <c r="N142" t="n">
-        <v>0.1184</v>
+        <v>0.0014</v>
       </c>
       <c r="O142" t="n">
-        <v>8.4</v>
+        <v>710</v>
       </c>
       <c r="P142" t="s">
-        <v>53</v>
+        <v>36</v>
       </c>
       <c r="Q142" t="s">
-        <v>760</v>
+        <v>37</v>
       </c>
       <c r="R142" t="s">
-        <v>136</v>
+        <v>25</v>
       </c>
       <c r="S142" t="s">
         <v>761</v>
@@ -10918,1129 +11098,1137 @@
         <v>763</v>
       </c>
       <c r="C143" s="1" t="n">
-        <v>44647</v>
+        <v>44641</v>
       </c>
       <c r="D143" t="s">
         <v>764</v>
       </c>
       <c r="E143" t="s">
-        <v>53</v>
-      </c>
-      <c r="F143" t="s">
         <v>765</v>
       </c>
+      <c r="F143"/>
       <c r="G143" t="n">
-        <v>752</v>
-      </c>
-      <c r="H143" t="n">
-        <v>50453548</v>
-      </c>
-      <c r="I143" t="n">
-        <v>9258.772</v>
-      </c>
+        <v>70</v>
+      </c>
+      <c r="H143"/>
+      <c r="I143"/>
       <c r="J143" t="n">
-        <v>9306</v>
+        <v>89400</v>
       </c>
       <c r="K143" t="n">
-        <v>1.708</v>
+        <v>16.393</v>
       </c>
       <c r="L143" t="n">
-        <v>26902</v>
+        <v>89400</v>
       </c>
       <c r="M143" t="n">
-        <v>4.937</v>
+        <v>16.393</v>
       </c>
       <c r="N143" t="n">
-        <v>0.328</v>
+        <v>0.1184</v>
       </c>
       <c r="O143" t="n">
-        <v>3</v>
+        <v>8.4</v>
       </c>
       <c r="P143" t="s">
         <v>53</v>
       </c>
       <c r="Q143" t="s">
-        <v>764</v>
+        <v>766</v>
       </c>
       <c r="R143" t="s">
-        <v>61</v>
+        <v>136</v>
       </c>
       <c r="S143" t="s">
-        <v>766</v>
+        <v>767</v>
       </c>
     </row>
     <row r="144">
       <c r="A144" t="s">
-        <v>767</v>
+        <v>768</v>
       </c>
       <c r="B144" t="s">
-        <v>768</v>
+        <v>769</v>
       </c>
       <c r="C144" s="1" t="n">
         <v>44647</v>
       </c>
       <c r="D144" t="s">
-        <v>769</v>
+        <v>770</v>
       </c>
       <c r="E144" t="s">
-        <v>770</v>
+        <v>53</v>
       </c>
       <c r="F144" t="s">
         <v>771</v>
       </c>
       <c r="G144" t="n">
-        <v>767</v>
+        <v>752</v>
       </c>
       <c r="H144" t="n">
-        <v>4746660</v>
+        <v>50453548</v>
       </c>
       <c r="I144" t="n">
-        <v>2283.45</v>
+        <v>9258.772</v>
       </c>
       <c r="J144" t="n">
-        <v>5466</v>
+        <v>9306</v>
       </c>
       <c r="K144" t="n">
-        <v>2.629</v>
+        <v>1.708</v>
       </c>
       <c r="L144" t="n">
-        <v>13366</v>
+        <v>26902</v>
       </c>
       <c r="M144" t="n">
-        <v>6.43</v>
+        <v>4.937</v>
       </c>
       <c r="N144" t="n">
-        <v>0.21</v>
+        <v>0.328</v>
       </c>
       <c r="O144" t="n">
-        <v>4.8</v>
+        <v>3</v>
       </c>
       <c r="P144" t="s">
-        <v>772</v>
+        <v>53</v>
       </c>
       <c r="Q144" t="s">
-        <v>769</v>
+        <v>770</v>
       </c>
       <c r="R144" t="s">
         <v>61</v>
       </c>
       <c r="S144" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
     </row>
     <row r="145">
       <c r="A145" t="s">
+        <v>773</v>
+      </c>
+      <c r="B145" t="s">
         <v>774</v>
       </c>
-      <c r="B145" t="s">
+      <c r="C145" s="1" t="n">
+        <v>44647</v>
+      </c>
+      <c r="D145" t="s">
         <v>775</v>
       </c>
-      <c r="C145" s="1" t="n">
-        <v>44632</v>
-      </c>
-      <c r="D145" t="s">
-        <v>35</v>
-      </c>
       <c r="E145" t="s">
-        <v>36</v>
-      </c>
-      <c r="F145"/>
+        <v>776</v>
+      </c>
+      <c r="F145" t="s">
+        <v>777</v>
+      </c>
       <c r="G145" t="n">
-        <v>1</v>
+        <v>767</v>
       </c>
       <c r="H145" t="n">
-        <v>400466</v>
+        <v>4746660</v>
       </c>
       <c r="I145" t="n">
-        <v>24.479</v>
-      </c>
-      <c r="J145"/>
-      <c r="K145"/>
-      <c r="L145"/>
-      <c r="M145"/>
-      <c r="N145"/>
-      <c r="O145"/>
+        <v>2283.45</v>
+      </c>
+      <c r="J145" t="n">
+        <v>5466</v>
+      </c>
+      <c r="K145" t="n">
+        <v>2.629</v>
+      </c>
+      <c r="L145" t="n">
+        <v>13366</v>
+      </c>
+      <c r="M145" t="n">
+        <v>6.43</v>
+      </c>
+      <c r="N145" t="n">
+        <v>0.21</v>
+      </c>
+      <c r="O145" t="n">
+        <v>4.8</v>
+      </c>
       <c r="P145" t="s">
-        <v>36</v>
+        <v>778</v>
       </c>
       <c r="Q145" t="s">
-        <v>37</v>
+        <v>775</v>
       </c>
       <c r="R145" t="s">
-        <v>25</v>
+        <v>61</v>
       </c>
       <c r="S145" t="s">
-        <v>776</v>
+        <v>779</v>
       </c>
     </row>
     <row r="146">
       <c r="A146" t="s">
-        <v>777</v>
+        <v>780</v>
       </c>
       <c r="B146" t="s">
-        <v>778</v>
+        <v>781</v>
       </c>
       <c r="C146" s="1" t="n">
-        <v>44648</v>
+        <v>44632</v>
       </c>
       <c r="D146" t="s">
-        <v>779</v>
+        <v>35</v>
       </c>
       <c r="E146" t="s">
-        <v>780</v>
-      </c>
-      <c r="F146" t="s">
-        <v>781</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="F146"/>
       <c r="G146" t="n">
-        <v>748</v>
+        <v>1</v>
       </c>
       <c r="H146" t="n">
-        <v>23757304</v>
+        <v>400466</v>
       </c>
       <c r="I146" t="n">
-        <v>395.678</v>
-      </c>
-      <c r="J146" t="n">
-        <v>12942</v>
-      </c>
-      <c r="K146" t="n">
-        <v>0.216</v>
-      </c>
-      <c r="L146" t="n">
-        <v>22477</v>
-      </c>
-      <c r="M146" t="n">
-        <v>0.374</v>
-      </c>
+        <v>24.479</v>
+      </c>
+      <c r="J146"/>
+      <c r="K146"/>
+      <c r="L146"/>
+      <c r="M146"/>
       <c r="N146"/>
       <c r="O146"/>
       <c r="P146" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q146" t="s">
+        <v>37</v>
+      </c>
+      <c r="R146" t="s">
+        <v>25</v>
+      </c>
+      <c r="S146" t="s">
         <v>782</v>
-      </c>
-      <c r="Q146" t="s">
-        <v>779</v>
-      </c>
-      <c r="R146" t="s">
-        <v>45</v>
-      </c>
-      <c r="S146" t="s">
-        <v>783</v>
       </c>
     </row>
     <row r="147">
       <c r="A147" t="s">
+        <v>783</v>
+      </c>
+      <c r="B147" t="s">
         <v>784</v>
       </c>
-      <c r="B147" t="s">
+      <c r="C147" s="1" t="n">
+        <v>44648</v>
+      </c>
+      <c r="D147" t="s">
         <v>785</v>
       </c>
-      <c r="C147" s="1" t="n">
-        <v>44647</v>
-      </c>
-      <c r="D147" t="s">
+      <c r="E147" t="s">
         <v>786</v>
       </c>
-      <c r="E147" t="s">
+      <c r="F147" t="s">
         <v>787</v>
       </c>
-      <c r="F147" t="s">
+      <c r="G147" t="n">
+        <v>748</v>
+      </c>
+      <c r="H147" t="n">
+        <v>23757304</v>
+      </c>
+      <c r="I147" t="n">
+        <v>395.678</v>
+      </c>
+      <c r="J147" t="n">
+        <v>12942</v>
+      </c>
+      <c r="K147" t="n">
+        <v>0.216</v>
+      </c>
+      <c r="L147" t="n">
+        <v>22477</v>
+      </c>
+      <c r="M147" t="n">
+        <v>0.374</v>
+      </c>
+      <c r="N147" t="n">
+        <v>0.0575</v>
+      </c>
+      <c r="O147" t="n">
+        <v>17.4</v>
+      </c>
+      <c r="P147" t="s">
         <v>788</v>
       </c>
-      <c r="G147" t="n">
-        <v>779</v>
-      </c>
-      <c r="H147" t="n">
-        <v>85330343</v>
-      </c>
-      <c r="I147" t="n">
-        <v>1663.191</v>
-      </c>
-      <c r="J147" t="n">
-        <v>334483</v>
-      </c>
-      <c r="K147" t="n">
-        <v>6.519</v>
-      </c>
-      <c r="L147" t="n">
-        <v>539005</v>
-      </c>
-      <c r="M147" t="n">
-        <v>10.506</v>
-      </c>
-      <c r="N147" t="n">
-        <v>0.6415</v>
-      </c>
-      <c r="O147" t="n">
-        <v>1.6</v>
-      </c>
-      <c r="P147" t="s">
-        <v>789</v>
-      </c>
       <c r="Q147" t="s">
-        <v>790</v>
+        <v>785</v>
       </c>
       <c r="R147" t="s">
         <v>45</v>
       </c>
       <c r="S147" t="s">
-        <v>791</v>
+        <v>789</v>
       </c>
     </row>
     <row r="148">
       <c r="A148" t="s">
+        <v>790</v>
+      </c>
+      <c r="B148" t="s">
+        <v>791</v>
+      </c>
+      <c r="C148" s="1" t="n">
+        <v>44647</v>
+      </c>
+      <c r="D148" t="s">
         <v>792</v>
       </c>
-      <c r="B148" t="s">
+      <c r="E148" t="s">
         <v>793</v>
       </c>
-      <c r="C148" s="1" t="n">
-        <v>44648</v>
-      </c>
-      <c r="D148" t="s">
-        <v>35</v>
-      </c>
-      <c r="E148" t="s">
-        <v>36</v>
-      </c>
-      <c r="F148"/>
+      <c r="F148" t="s">
+        <v>794</v>
+      </c>
       <c r="G148" t="n">
-        <v>162</v>
+        <v>779</v>
       </c>
       <c r="H148" t="n">
-        <v>358442</v>
+        <v>85330343</v>
       </c>
       <c r="I148" t="n">
-        <v>31.494</v>
-      </c>
-      <c r="J148"/>
-      <c r="K148"/>
+        <v>1663.191</v>
+      </c>
+      <c r="J148" t="n">
+        <v>334483</v>
+      </c>
+      <c r="K148" t="n">
+        <v>6.519</v>
+      </c>
       <c r="L148" t="n">
-        <v>909</v>
+        <v>539005</v>
       </c>
       <c r="M148" t="n">
-        <v>0.08</v>
-      </c>
-      <c r="N148"/>
-      <c r="O148"/>
+        <v>10.506</v>
+      </c>
+      <c r="N148" t="n">
+        <v>0.6415</v>
+      </c>
+      <c r="O148" t="n">
+        <v>1.6</v>
+      </c>
       <c r="P148" t="s">
-        <v>36</v>
+        <v>795</v>
       </c>
       <c r="Q148" t="s">
-        <v>37</v>
+        <v>796</v>
       </c>
       <c r="R148" t="s">
-        <v>25</v>
+        <v>45</v>
       </c>
       <c r="S148" t="s">
-        <v>794</v>
+        <v>797</v>
       </c>
     </row>
     <row r="149">
       <c r="A149" t="s">
-        <v>795</v>
+        <v>798</v>
       </c>
       <c r="B149" t="s">
-        <v>796</v>
+        <v>799</v>
       </c>
       <c r="C149" s="1" t="n">
-        <v>44645</v>
+        <v>44648</v>
       </c>
       <c r="D149" t="s">
-        <v>797</v>
+        <v>35</v>
       </c>
       <c r="E149" t="s">
-        <v>53</v>
+        <v>36</v>
       </c>
       <c r="F149"/>
       <c r="G149" t="n">
-        <v>741</v>
+        <v>162</v>
       </c>
       <c r="H149" t="n">
-        <v>88147343</v>
+        <v>358442</v>
       </c>
       <c r="I149" t="n">
-        <v>1885.698</v>
-      </c>
-      <c r="J149" t="n">
-        <v>60487</v>
-      </c>
-      <c r="K149" t="n">
-        <v>1.294</v>
-      </c>
+        <v>31.494</v>
+      </c>
+      <c r="J149"/>
+      <c r="K149"/>
       <c r="L149" t="n">
-        <v>83657</v>
+        <v>909</v>
       </c>
       <c r="M149" t="n">
-        <v>1.79</v>
+        <v>0.08</v>
       </c>
       <c r="N149" t="n">
-        <v>0.191</v>
+        <v>0.0134</v>
       </c>
       <c r="O149" t="n">
-        <v>5.2</v>
+        <v>74.9</v>
       </c>
       <c r="P149" t="s">
-        <v>798</v>
+        <v>36</v>
       </c>
       <c r="Q149" t="s">
-        <v>797</v>
+        <v>37</v>
       </c>
       <c r="R149" t="s">
-        <v>61</v>
+        <v>25</v>
       </c>
       <c r="S149" t="s">
-        <v>799</v>
+        <v>800</v>
       </c>
     </row>
     <row r="150">
       <c r="A150" t="s">
-        <v>800</v>
+        <v>801</v>
       </c>
       <c r="B150" t="s">
-        <v>801</v>
+        <v>802</v>
       </c>
       <c r="C150" s="1" t="n">
-        <v>44647</v>
+        <v>44645</v>
       </c>
       <c r="D150" t="s">
-        <v>802</v>
+        <v>803</v>
       </c>
       <c r="E150" t="s">
-        <v>803</v>
+        <v>53</v>
       </c>
       <c r="F150"/>
       <c r="G150" t="n">
-        <v>762</v>
+        <v>741</v>
       </c>
       <c r="H150" t="n">
-        <v>7535729</v>
+        <v>88147343</v>
       </c>
       <c r="I150" t="n">
-        <v>350.543</v>
+        <v>1885.698</v>
       </c>
       <c r="J150" t="n">
-        <v>5048</v>
+        <v>60487</v>
       </c>
       <c r="K150" t="n">
-        <v>0.235</v>
+        <v>1.294</v>
       </c>
       <c r="L150" t="n">
-        <v>4573</v>
+        <v>83657</v>
       </c>
       <c r="M150" t="n">
-        <v>0.213</v>
+        <v>1.79</v>
       </c>
       <c r="N150" t="n">
-        <v>0.0841</v>
+        <v>0.191</v>
       </c>
       <c r="O150" t="n">
-        <v>11.9</v>
+        <v>5.2</v>
       </c>
       <c r="P150" t="s">
+        <v>804</v>
+      </c>
+      <c r="Q150" t="s">
         <v>803</v>
-      </c>
-      <c r="Q150" t="s">
-        <v>802</v>
       </c>
       <c r="R150" t="s">
         <v>61</v>
       </c>
       <c r="S150" t="s">
-        <v>804</v>
+        <v>805</v>
       </c>
     </row>
     <row r="151">
       <c r="A151" t="s">
-        <v>805</v>
+        <v>806</v>
       </c>
       <c r="B151" t="s">
-        <v>806</v>
+        <v>807</v>
       </c>
       <c r="C151" s="1" t="n">
-        <v>44605</v>
+        <v>44647</v>
       </c>
       <c r="D151" t="s">
-        <v>35</v>
+        <v>808</v>
       </c>
       <c r="E151" t="s">
-        <v>36</v>
+        <v>809</v>
       </c>
       <c r="F151"/>
       <c r="G151" t="n">
-        <v>1</v>
+        <v>762</v>
       </c>
       <c r="H151" t="n">
-        <v>562941</v>
+        <v>7535729</v>
       </c>
       <c r="I151" t="n">
-        <v>12.535</v>
-      </c>
-      <c r="J151"/>
-      <c r="K151"/>
-      <c r="L151"/>
-      <c r="M151"/>
-      <c r="N151"/>
-      <c r="O151"/>
+        <v>350.543</v>
+      </c>
+      <c r="J151" t="n">
+        <v>5048</v>
+      </c>
+      <c r="K151" t="n">
+        <v>0.235</v>
+      </c>
+      <c r="L151" t="n">
+        <v>4573</v>
+      </c>
+      <c r="M151" t="n">
+        <v>0.213</v>
+      </c>
+      <c r="N151" t="n">
+        <v>0.0841</v>
+      </c>
+      <c r="O151" t="n">
+        <v>11.9</v>
+      </c>
       <c r="P151" t="s">
-        <v>36</v>
+        <v>809</v>
       </c>
       <c r="Q151" t="s">
-        <v>37</v>
+        <v>808</v>
       </c>
       <c r="R151" t="s">
-        <v>25</v>
+        <v>61</v>
       </c>
       <c r="S151" t="s">
-        <v>807</v>
+        <v>810</v>
       </c>
     </row>
     <row r="152">
       <c r="A152" t="s">
-        <v>808</v>
+        <v>811</v>
       </c>
       <c r="B152" t="s">
-        <v>809</v>
+        <v>812</v>
       </c>
       <c r="C152" s="1" t="n">
-        <v>44644</v>
+        <v>44605</v>
       </c>
       <c r="D152" t="s">
-        <v>810</v>
+        <v>35</v>
       </c>
       <c r="E152" t="s">
-        <v>811</v>
+        <v>36</v>
       </c>
       <c r="F152"/>
       <c r="G152" t="n">
-        <v>206</v>
+        <v>1</v>
       </c>
       <c r="H152" t="n">
-        <v>81647</v>
+        <v>562941</v>
       </c>
       <c r="I152" t="n">
-        <v>137.964</v>
-      </c>
-      <c r="J152" t="n">
-        <v>177</v>
-      </c>
-      <c r="K152" t="n">
-        <v>0.299</v>
-      </c>
-      <c r="L152" t="n">
-        <v>31</v>
-      </c>
-      <c r="M152" t="n">
-        <v>0.052</v>
-      </c>
-      <c r="N152" t="n">
-        <v>0.137</v>
-      </c>
-      <c r="O152" t="n">
-        <v>7.3</v>
-      </c>
+        <v>12.535</v>
+      </c>
+      <c r="J152"/>
+      <c r="K152"/>
+      <c r="L152"/>
+      <c r="M152"/>
+      <c r="N152"/>
+      <c r="O152"/>
       <c r="P152" t="s">
-        <v>811</v>
+        <v>36</v>
       </c>
       <c r="Q152" t="s">
-        <v>810</v>
+        <v>37</v>
       </c>
       <c r="R152" t="s">
         <v>25</v>
       </c>
       <c r="S152" t="s">
-        <v>812</v>
+        <v>813</v>
       </c>
     </row>
     <row r="153">
       <c r="A153" t="s">
-        <v>813</v>
+        <v>814</v>
       </c>
       <c r="B153" t="s">
-        <v>814</v>
+        <v>815</v>
       </c>
       <c r="C153" s="1" t="n">
-        <v>44640</v>
+        <v>44644</v>
       </c>
       <c r="D153" t="s">
-        <v>815</v>
+        <v>816</v>
       </c>
       <c r="E153" t="s">
-        <v>816</v>
+        <v>817</v>
       </c>
       <c r="F153"/>
       <c r="G153" t="n">
-        <v>630</v>
+        <v>206</v>
       </c>
       <c r="H153" t="n">
-        <v>18121775</v>
+        <v>81647</v>
       </c>
       <c r="I153" t="n">
-        <v>1783.611</v>
+        <v>137.964</v>
       </c>
       <c r="J153" t="n">
-        <v>5752</v>
+        <v>177</v>
       </c>
       <c r="K153" t="n">
-        <v>0.566</v>
+        <v>0.299</v>
       </c>
       <c r="L153" t="n">
-        <v>5752</v>
+        <v>31</v>
       </c>
       <c r="M153" t="n">
-        <v>0.566</v>
+        <v>0.052</v>
       </c>
       <c r="N153" t="n">
-        <v>0.2263</v>
+        <v>0.137</v>
       </c>
       <c r="O153" t="n">
-        <v>4.4</v>
+        <v>7.3</v>
       </c>
       <c r="P153" t="s">
         <v>817</v>
       </c>
       <c r="Q153" t="s">
+        <v>816</v>
+      </c>
+      <c r="R153" t="s">
+        <v>25</v>
+      </c>
+      <c r="S153" t="s">
         <v>818</v>
-      </c>
-      <c r="R153" t="s">
-        <v>61</v>
-      </c>
-      <c r="S153" t="s">
-        <v>819</v>
       </c>
     </row>
     <row r="154">
       <c r="A154" t="s">
+        <v>819</v>
+      </c>
+      <c r="B154" t="s">
         <v>820</v>
       </c>
-      <c r="B154" t="s">
+      <c r="C154" s="1" t="n">
+        <v>44640</v>
+      </c>
+      <c r="D154" t="s">
         <v>821</v>
       </c>
-      <c r="C154" s="1" t="n">
-        <v>44647</v>
-      </c>
-      <c r="D154" t="s">
-        <v>522</v>
-      </c>
       <c r="E154" t="s">
-        <v>523</v>
+        <v>822</v>
       </c>
       <c r="F154"/>
       <c r="G154" t="n">
-        <v>674</v>
+        <v>630</v>
       </c>
       <c r="H154" t="n">
-        <v>20157569</v>
+        <v>18121775</v>
       </c>
       <c r="I154" t="n">
-        <v>2312.843</v>
+        <v>1783.611</v>
       </c>
       <c r="J154" t="n">
-        <v>13353</v>
+        <v>5752</v>
       </c>
       <c r="K154" t="n">
-        <v>1.532</v>
+        <v>0.566</v>
       </c>
       <c r="L154" t="n">
-        <v>45374</v>
+        <v>5752</v>
       </c>
       <c r="M154" t="n">
-        <v>5.206</v>
+        <v>0.566</v>
       </c>
       <c r="N154" t="n">
-        <v>0.44</v>
+        <v>0.2263</v>
       </c>
       <c r="O154" t="n">
-        <v>2.3</v>
+        <v>4.4</v>
       </c>
       <c r="P154" t="s">
-        <v>523</v>
+        <v>823</v>
       </c>
       <c r="Q154" t="s">
-        <v>524</v>
+        <v>824</v>
       </c>
       <c r="R154" t="s">
         <v>61</v>
       </c>
       <c r="S154" t="s">
-        <v>822</v>
+        <v>825</v>
       </c>
     </row>
     <row r="155">
       <c r="A155" t="s">
-        <v>823</v>
+        <v>826</v>
       </c>
       <c r="B155" t="s">
-        <v>824</v>
+        <v>827</v>
       </c>
       <c r="C155" s="1" t="n">
-        <v>44632</v>
+        <v>44647</v>
       </c>
       <c r="D155" t="s">
-        <v>21</v>
+        <v>522</v>
       </c>
       <c r="E155" t="s">
-        <v>22</v>
+        <v>523</v>
       </c>
       <c r="F155"/>
       <c r="G155" t="n">
-        <v>2</v>
+        <v>674</v>
       </c>
       <c r="H155" t="n">
-        <v>158382</v>
+        <v>20157569</v>
       </c>
       <c r="I155" t="n">
-        <v>8.666</v>
-      </c>
-      <c r="J155"/>
-      <c r="K155"/>
+        <v>2312.843</v>
+      </c>
+      <c r="J155" t="n">
+        <v>13353</v>
+      </c>
+      <c r="K155" t="n">
+        <v>1.532</v>
+      </c>
       <c r="L155" t="n">
-        <v>157</v>
+        <v>45374</v>
       </c>
       <c r="M155" t="n">
-        <v>0.009</v>
+        <v>5.206</v>
       </c>
       <c r="N155" t="n">
-        <v>0.333</v>
+        <v>0.44</v>
       </c>
       <c r="O155" t="n">
-        <v>3</v>
+        <v>2.3</v>
       </c>
       <c r="P155" t="s">
-        <v>23</v>
+        <v>523</v>
       </c>
       <c r="Q155" t="s">
-        <v>24</v>
+        <v>524</v>
       </c>
       <c r="R155" t="s">
-        <v>25</v>
+        <v>61</v>
       </c>
       <c r="S155" t="s">
-        <v>26</v>
+        <v>828</v>
       </c>
     </row>
     <row r="156">
       <c r="A156" t="s">
-        <v>825</v>
+        <v>829</v>
       </c>
       <c r="B156" t="s">
-        <v>826</v>
+        <v>830</v>
       </c>
       <c r="C156" s="1" t="n">
-        <v>44648</v>
+        <v>44632</v>
       </c>
       <c r="D156" t="s">
-        <v>827</v>
+        <v>21</v>
       </c>
       <c r="E156" t="s">
-        <v>828</v>
+        <v>22</v>
       </c>
       <c r="F156"/>
       <c r="G156" t="n">
-        <v>802</v>
+        <v>2</v>
       </c>
       <c r="H156" t="n">
-        <v>6931880</v>
+        <v>158382</v>
       </c>
       <c r="I156" t="n">
-        <v>290.584</v>
-      </c>
-      <c r="J156" t="n">
-        <v>20974</v>
-      </c>
-      <c r="K156" t="n">
-        <v>0.879</v>
-      </c>
+        <v>8.666</v>
+      </c>
+      <c r="J156"/>
+      <c r="K156"/>
       <c r="L156" t="n">
-        <v>21321</v>
+        <v>157</v>
       </c>
       <c r="M156" t="n">
-        <v>0.894</v>
-      </c>
-      <c r="N156"/>
-      <c r="O156"/>
+        <v>0.009</v>
+      </c>
+      <c r="N156" t="n">
+        <v>0.333</v>
+      </c>
+      <c r="O156" t="n">
+        <v>3</v>
+      </c>
       <c r="P156" t="s">
-        <v>828</v>
+        <v>23</v>
       </c>
       <c r="Q156" t="s">
-        <v>827</v>
+        <v>24</v>
       </c>
       <c r="R156" t="s">
-        <v>45</v>
+        <v>25</v>
       </c>
       <c r="S156" t="s">
-        <v>829</v>
+        <v>26</v>
       </c>
     </row>
     <row r="157">
       <c r="A157" t="s">
-        <v>830</v>
+        <v>831</v>
       </c>
       <c r="B157" t="s">
-        <v>831</v>
+        <v>832</v>
       </c>
       <c r="C157" s="1" t="n">
-        <v>44610</v>
+        <v>44648</v>
       </c>
       <c r="D157" t="s">
-        <v>832</v>
+        <v>833</v>
       </c>
       <c r="E157" t="s">
-        <v>53</v>
+        <v>834</v>
       </c>
       <c r="F157"/>
       <c r="G157" t="n">
-        <v>2</v>
+        <v>802</v>
       </c>
       <c r="H157" t="n">
-        <v>455776</v>
+        <v>6931880</v>
       </c>
       <c r="I157" t="n">
-        <v>7.411</v>
-      </c>
-      <c r="J157"/>
-      <c r="K157"/>
+        <v>290.584</v>
+      </c>
+      <c r="J157" t="n">
+        <v>20974</v>
+      </c>
+      <c r="K157" t="n">
+        <v>0.879</v>
+      </c>
       <c r="L157" t="n">
-        <v>1004</v>
+        <v>21321</v>
       </c>
       <c r="M157" t="n">
-        <v>0.016</v>
+        <v>0.894</v>
       </c>
       <c r="N157" t="n">
-        <v>0.0161</v>
+        <v>0.006</v>
       </c>
       <c r="O157" t="n">
-        <v>62.2</v>
+        <v>167.1</v>
       </c>
       <c r="P157" t="s">
-        <v>36</v>
+        <v>834</v>
       </c>
       <c r="Q157" t="s">
         <v>833</v>
       </c>
       <c r="R157" t="s">
-        <v>25</v>
+        <v>45</v>
       </c>
       <c r="S157" t="s">
-        <v>834</v>
+        <v>835</v>
       </c>
     </row>
     <row r="158">
       <c r="A158" t="s">
-        <v>835</v>
+        <v>836</v>
       </c>
       <c r="B158" t="s">
-        <v>836</v>
+        <v>837</v>
       </c>
       <c r="C158" s="1" t="n">
-        <v>44625</v>
+        <v>44610</v>
       </c>
       <c r="D158" t="s">
-        <v>837</v>
+        <v>838</v>
       </c>
       <c r="E158" t="s">
-        <v>838</v>
+        <v>53</v>
       </c>
       <c r="F158"/>
       <c r="G158" t="n">
-        <v>791</v>
+        <v>2</v>
       </c>
       <c r="H158" t="n">
-        <v>21377196</v>
+        <v>455776</v>
       </c>
       <c r="I158" t="n">
-        <v>305.603</v>
-      </c>
-      <c r="J158" t="n">
-        <v>40281</v>
-      </c>
-      <c r="K158" t="n">
-        <v>0.576</v>
-      </c>
+        <v>7.411</v>
+      </c>
+      <c r="J158"/>
+      <c r="K158"/>
       <c r="L158" t="n">
-        <v>61456</v>
+        <v>1004</v>
       </c>
       <c r="M158" t="n">
-        <v>0.879</v>
+        <v>0.016</v>
       </c>
       <c r="N158" t="n">
-        <v>0.3651</v>
+        <v>0.0161</v>
       </c>
       <c r="O158" t="n">
-        <v>2.7</v>
+        <v>62.2</v>
       </c>
       <c r="P158" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q158" t="s">
         <v>839</v>
       </c>
-      <c r="Q158" t="s">
+      <c r="R158" t="s">
+        <v>25</v>
+      </c>
+      <c r="S158" t="s">
         <v>840</v>
-      </c>
-      <c r="R158" t="s">
-        <v>61</v>
-      </c>
-      <c r="S158" t="s">
-        <v>841</v>
       </c>
     </row>
     <row r="159">
       <c r="A159" t="s">
+        <v>841</v>
+      </c>
+      <c r="B159" t="s">
         <v>842</v>
       </c>
-      <c r="B159" t="s">
+      <c r="C159" s="1" t="n">
+        <v>44625</v>
+      </c>
+      <c r="D159" t="s">
         <v>843</v>
       </c>
-      <c r="C159" s="1" t="n">
-        <v>44632</v>
-      </c>
-      <c r="D159" t="s">
+      <c r="E159" t="s">
         <v>844</v>
-      </c>
-      <c r="E159" t="s">
-        <v>53</v>
       </c>
       <c r="F159"/>
       <c r="G159" t="n">
-        <v>32</v>
+        <v>791</v>
       </c>
       <c r="H159" t="n">
-        <v>252951</v>
+        <v>21377196</v>
       </c>
       <c r="I159" t="n">
-        <v>188.225</v>
-      </c>
-      <c r="J159"/>
-      <c r="K159"/>
+        <v>305.603</v>
+      </c>
+      <c r="J159" t="n">
+        <v>40281</v>
+      </c>
+      <c r="K159" t="n">
+        <v>0.576</v>
+      </c>
       <c r="L159" t="n">
-        <v>314</v>
+        <v>61456</v>
       </c>
       <c r="M159" t="n">
-        <v>0.234</v>
+        <v>0.879</v>
       </c>
       <c r="N159" t="n">
-        <v>0.0218</v>
+        <v>0.3651</v>
       </c>
       <c r="O159" t="n">
-        <v>45.8</v>
+        <v>2.7</v>
       </c>
       <c r="P159" t="s">
-        <v>53</v>
+        <v>845</v>
       </c>
       <c r="Q159" t="s">
-        <v>844</v>
+        <v>846</v>
       </c>
       <c r="R159" t="s">
-        <v>25</v>
+        <v>61</v>
       </c>
       <c r="S159" t="s">
-        <v>845</v>
+        <v>847</v>
       </c>
     </row>
     <row r="160">
       <c r="A160" t="s">
-        <v>846</v>
+        <v>848</v>
       </c>
       <c r="B160" t="s">
-        <v>847</v>
+        <v>849</v>
       </c>
       <c r="C160" s="1" t="n">
-        <v>44647</v>
+        <v>44632</v>
       </c>
       <c r="D160" t="s">
-        <v>848</v>
+        <v>850</v>
       </c>
       <c r="E160" t="s">
         <v>53</v>
       </c>
       <c r="F160"/>
       <c r="G160" t="n">
-        <v>743</v>
+        <v>32</v>
       </c>
       <c r="H160" t="n">
-        <v>716349</v>
+        <v>252951</v>
       </c>
       <c r="I160" t="n">
-        <v>84.493</v>
+        <v>188.225</v>
       </c>
       <c r="J160"/>
       <c r="K160"/>
       <c r="L160" t="n">
-        <v>931</v>
+        <v>314</v>
       </c>
       <c r="M160" t="n">
-        <v>0.11</v>
+        <v>0.234</v>
       </c>
       <c r="N160" t="n">
-        <v>0.006</v>
+        <v>0.0218</v>
       </c>
       <c r="O160" t="n">
-        <v>167.1</v>
+        <v>45.8</v>
       </c>
       <c r="P160" t="s">
-        <v>849</v>
+        <v>53</v>
       </c>
       <c r="Q160" t="s">
-        <v>848</v>
+        <v>850</v>
       </c>
       <c r="R160" t="s">
-        <v>61</v>
+        <v>25</v>
       </c>
       <c r="S160" t="s">
-        <v>850</v>
+        <v>851</v>
       </c>
     </row>
     <row r="161">
       <c r="A161" t="s">
-        <v>851</v>
+        <v>852</v>
       </c>
       <c r="B161" t="s">
-        <v>852</v>
+        <v>853</v>
       </c>
       <c r="C161" s="1" t="n">
         <v>44647</v>
       </c>
       <c r="D161" t="s">
-        <v>853</v>
+        <v>854</v>
       </c>
       <c r="E161" t="s">
         <v>53</v>
       </c>
       <c r="F161"/>
       <c r="G161" t="n">
-        <v>435</v>
+        <v>743</v>
       </c>
       <c r="H161" t="n">
-        <v>668817</v>
+        <v>716349</v>
       </c>
       <c r="I161" t="n">
-        <v>476.578</v>
-      </c>
-      <c r="J161" t="n">
-        <v>630</v>
-      </c>
-      <c r="K161" t="n">
-        <v>0.449</v>
-      </c>
+        <v>84.493</v>
+      </c>
+      <c r="J161"/>
+      <c r="K161"/>
       <c r="L161" t="n">
-        <v>1237</v>
+        <v>931</v>
       </c>
       <c r="M161" t="n">
-        <v>0.881</v>
+        <v>0.11</v>
       </c>
       <c r="N161" t="n">
-        <v>0.233</v>
+        <v>0.006</v>
       </c>
       <c r="O161" t="n">
-        <v>4.3</v>
+        <v>167.1</v>
       </c>
       <c r="P161" t="s">
-        <v>53</v>
+        <v>855</v>
       </c>
       <c r="Q161" t="s">
         <v>854</v>
       </c>
       <c r="R161" t="s">
-        <v>45</v>
+        <v>61</v>
       </c>
       <c r="S161" t="s">
-        <v>855</v>
+        <v>856</v>
       </c>
     </row>
     <row r="162">
       <c r="A162" t="s">
-        <v>856</v>
+        <v>857</v>
       </c>
       <c r="B162" t="s">
-        <v>857</v>
+        <v>858</v>
       </c>
       <c r="C162" s="1" t="n">
-        <v>44640</v>
+        <v>44647</v>
       </c>
       <c r="D162" t="s">
-        <v>858</v>
+        <v>859</v>
       </c>
       <c r="E162" t="s">
-        <v>859</v>
+        <v>53</v>
       </c>
       <c r="F162"/>
       <c r="G162" t="n">
-        <v>176</v>
+        <v>435</v>
       </c>
       <c r="H162" t="n">
-        <v>4500701</v>
+        <v>668817</v>
       </c>
       <c r="I162" t="n">
-        <v>377.077</v>
-      </c>
-      <c r="J162"/>
-      <c r="K162"/>
+        <v>476.578</v>
+      </c>
+      <c r="J162" t="n">
+        <v>630</v>
+      </c>
+      <c r="K162" t="n">
+        <v>0.449</v>
+      </c>
       <c r="L162" t="n">
-        <v>3667</v>
+        <v>1237</v>
       </c>
       <c r="M162" t="n">
-        <v>0.307</v>
+        <v>0.881</v>
       </c>
       <c r="N162" t="n">
-        <v>0.0208</v>
+        <v>0.233</v>
       </c>
       <c r="O162" t="n">
-        <v>48.1</v>
+        <v>4.3</v>
       </c>
       <c r="P162" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q162" t="s">
         <v>860</v>
-      </c>
-      <c r="Q162" t="s">
-        <v>861</v>
       </c>
       <c r="R162" t="s">
         <v>45</v>
       </c>
       <c r="S162" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
     </row>
     <row r="163">
       <c r="A163" t="s">
+        <v>862</v>
+      </c>
+      <c r="B163" t="s">
         <v>863</v>
       </c>
-      <c r="B163" t="s">
+      <c r="C163" s="1" t="n">
+        <v>44640</v>
+      </c>
+      <c r="D163" t="s">
         <v>864</v>
       </c>
-      <c r="C163" s="1" t="n">
-        <v>44643</v>
-      </c>
-      <c r="D163" t="s">
+      <c r="E163" t="s">
         <v>865</v>
-      </c>
-      <c r="E163" t="s">
-        <v>866</v>
       </c>
       <c r="F163"/>
       <c r="G163" t="n">
-        <v>727</v>
+        <v>176</v>
       </c>
       <c r="H163" t="n">
-        <v>151851543</v>
+        <v>4500701</v>
       </c>
       <c r="I163" t="n">
-        <v>1785.591</v>
-      </c>
-      <c r="J163" t="n">
-        <v>301014</v>
-      </c>
-      <c r="K163" t="n">
-        <v>3.54</v>
-      </c>
+        <v>377.077</v>
+      </c>
+      <c r="J163"/>
+      <c r="K163"/>
       <c r="L163" t="n">
-        <v>295374</v>
+        <v>3667</v>
       </c>
       <c r="M163" t="n">
-        <v>3.473</v>
+        <v>0.307</v>
       </c>
       <c r="N163" t="n">
-        <v>0.0582</v>
+        <v>0.0208</v>
       </c>
       <c r="O163" t="n">
-        <v>17.2</v>
+        <v>48.1</v>
       </c>
       <c r="P163" t="s">
         <v>866</v>
@@ -12049,7 +12237,7 @@
         <v>867</v>
       </c>
       <c r="R163" t="s">
-        <v>61</v>
+        <v>45</v>
       </c>
       <c r="S163" t="s">
         <v>868</v>
@@ -12063,92 +12251,100 @@
         <v>870</v>
       </c>
       <c r="C164" s="1" t="n">
-        <v>44648</v>
+        <v>44643</v>
       </c>
       <c r="D164" t="s">
-        <v>35</v>
+        <v>871</v>
       </c>
       <c r="E164" t="s">
-        <v>36</v>
+        <v>872</v>
       </c>
       <c r="F164"/>
       <c r="G164" t="n">
-        <v>632</v>
+        <v>727</v>
       </c>
       <c r="H164" t="n">
-        <v>2542633</v>
+        <v>151851543</v>
       </c>
       <c r="I164" t="n">
-        <v>53.957</v>
-      </c>
-      <c r="J164"/>
-      <c r="K164"/>
+        <v>1785.591</v>
+      </c>
+      <c r="J164" t="n">
+        <v>301014</v>
+      </c>
+      <c r="K164" t="n">
+        <v>3.54</v>
+      </c>
       <c r="L164" t="n">
-        <v>3578</v>
+        <v>295374</v>
       </c>
       <c r="M164" t="n">
-        <v>0.076</v>
-      </c>
-      <c r="N164"/>
-      <c r="O164"/>
+        <v>3.473</v>
+      </c>
+      <c r="N164" t="n">
+        <v>0.0582</v>
+      </c>
+      <c r="O164" t="n">
+        <v>17.2</v>
+      </c>
       <c r="P164" t="s">
-        <v>36</v>
+        <v>872</v>
       </c>
       <c r="Q164" t="s">
-        <v>37</v>
+        <v>873</v>
       </c>
       <c r="R164" t="s">
         <v>61</v>
       </c>
       <c r="S164" t="s">
-        <v>871</v>
+        <v>874</v>
       </c>
     </row>
     <row r="165">
       <c r="A165" t="s">
-        <v>872</v>
+        <v>875</v>
       </c>
       <c r="B165" t="s">
-        <v>873</v>
+        <v>876</v>
       </c>
       <c r="C165" s="1" t="n">
-        <v>44610</v>
+        <v>44648</v>
       </c>
       <c r="D165" t="s">
-        <v>874</v>
+        <v>35</v>
       </c>
       <c r="E165" t="s">
-        <v>875</v>
+        <v>36</v>
       </c>
       <c r="F165"/>
       <c r="G165" t="n">
-        <v>556</v>
+        <v>632</v>
       </c>
       <c r="H165" t="n">
-        <v>19288823</v>
+        <v>2542633</v>
       </c>
       <c r="I165" t="n">
-        <v>443.76</v>
+        <v>53.957</v>
       </c>
       <c r="J165"/>
       <c r="K165"/>
       <c r="L165" t="n">
-        <v>52561</v>
+        <v>3578</v>
       </c>
       <c r="M165" t="n">
-        <v>1.209</v>
+        <v>0.076</v>
       </c>
       <c r="N165" t="n">
-        <v>0.6027</v>
+        <v>0.004</v>
       </c>
       <c r="O165" t="n">
-        <v>1.7</v>
+        <v>248</v>
       </c>
       <c r="P165" t="s">
-        <v>875</v>
+        <v>36</v>
       </c>
       <c r="Q165" t="s">
-        <v>876</v>
+        <v>37</v>
       </c>
       <c r="R165" t="s">
         <v>61</v>
@@ -12165,7 +12361,7 @@
         <v>879</v>
       </c>
       <c r="C166" s="1" t="n">
-        <v>44648</v>
+        <v>44610</v>
       </c>
       <c r="D166" t="s">
         <v>880</v>
@@ -12175,28 +12371,28 @@
       </c>
       <c r="F166"/>
       <c r="G166" t="n">
-        <v>759</v>
+        <v>556</v>
       </c>
       <c r="H166" t="n">
-        <v>147145013</v>
+        <v>19288823</v>
       </c>
       <c r="I166" t="n">
-        <v>14727.634</v>
-      </c>
-      <c r="J166" t="n">
-        <v>229355</v>
-      </c>
-      <c r="K166" t="n">
-        <v>22.956</v>
-      </c>
+        <v>443.76</v>
+      </c>
+      <c r="J166"/>
+      <c r="K166"/>
       <c r="L166" t="n">
-        <v>300191</v>
+        <v>52561</v>
       </c>
       <c r="M166" t="n">
-        <v>30.046</v>
-      </c>
-      <c r="N166"/>
-      <c r="O166"/>
+        <v>1.209</v>
+      </c>
+      <c r="N166" t="n">
+        <v>0.6027</v>
+      </c>
+      <c r="O166" t="n">
+        <v>1.7</v>
+      </c>
       <c r="P166" t="s">
         <v>881</v>
       </c>
@@ -12218,7 +12414,7 @@
         <v>885</v>
       </c>
       <c r="C167" s="1" t="n">
-        <v>44647</v>
+        <v>44648</v>
       </c>
       <c r="D167" t="s">
         <v>886</v>
@@ -12228,93 +12424,97 @@
       </c>
       <c r="F167"/>
       <c r="G167" t="n">
-        <v>725</v>
+        <v>759</v>
       </c>
       <c r="H167" t="n">
-        <v>483762402</v>
+        <v>147145013</v>
       </c>
       <c r="I167" t="n">
-        <v>7092.551</v>
+        <v>14727.634</v>
       </c>
       <c r="J167" t="n">
-        <v>617522</v>
+        <v>229355</v>
       </c>
       <c r="K167" t="n">
-        <v>9.054</v>
+        <v>22.956</v>
       </c>
       <c r="L167" t="n">
-        <v>740542</v>
+        <v>300191</v>
       </c>
       <c r="M167" t="n">
-        <v>10.857</v>
-      </c>
-      <c r="N167"/>
-      <c r="O167"/>
+        <v>30.046</v>
+      </c>
+      <c r="N167" t="n">
+        <v>0.0011</v>
+      </c>
+      <c r="O167" t="n">
+        <v>902.6</v>
+      </c>
       <c r="P167" t="s">
+        <v>887</v>
+      </c>
+      <c r="Q167" t="s">
         <v>888</v>
-      </c>
-      <c r="Q167" t="s">
-        <v>889</v>
       </c>
       <c r="R167" t="s">
         <v>61</v>
       </c>
       <c r="S167" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
     </row>
     <row r="168">
       <c r="A168" t="s">
+        <v>890</v>
+      </c>
+      <c r="B168" t="s">
         <v>891</v>
       </c>
-      <c r="B168" t="s">
+      <c r="C168" s="1" t="n">
+        <v>44647</v>
+      </c>
+      <c r="D168" t="s">
         <v>892</v>
       </c>
-      <c r="C168" s="1" t="n">
-        <v>44642</v>
-      </c>
-      <c r="D168" t="s">
+      <c r="E168" t="s">
         <v>893</v>
-      </c>
-      <c r="E168" t="s">
-        <v>894</v>
       </c>
       <c r="F168"/>
       <c r="G168" t="n">
-        <v>752</v>
+        <v>725</v>
       </c>
       <c r="H168" t="n">
-        <v>842683453</v>
+        <v>483762402</v>
       </c>
       <c r="I168" t="n">
-        <v>2531.226</v>
+        <v>7092.551</v>
       </c>
       <c r="J168" t="n">
-        <v>958496</v>
+        <v>617522</v>
       </c>
       <c r="K168" t="n">
-        <v>2.879</v>
+        <v>9.054</v>
       </c>
       <c r="L168" t="n">
-        <v>834280</v>
+        <v>740542</v>
       </c>
       <c r="M168" t="n">
-        <v>2.506</v>
+        <v>10.857</v>
       </c>
       <c r="N168" t="n">
-        <v>0.022</v>
+        <v>0.1162</v>
       </c>
       <c r="O168" t="n">
-        <v>45.5</v>
+        <v>8.6</v>
       </c>
       <c r="P168" t="s">
         <v>894</v>
       </c>
       <c r="Q168" t="s">
-        <v>893</v>
+        <v>895</v>
       </c>
       <c r="R168" t="s">
-        <v>895</v>
+        <v>61</v>
       </c>
       <c r="S168" t="s">
         <v>896</v>
@@ -12328,310 +12528,371 @@
         <v>898</v>
       </c>
       <c r="C169" s="1" t="n">
-        <v>44647</v>
+        <v>44644</v>
       </c>
       <c r="D169" t="s">
-        <v>899</v>
+        <v>702</v>
       </c>
       <c r="E169" t="s">
-        <v>237</v>
+        <v>703</v>
       </c>
       <c r="F169"/>
       <c r="G169" t="n">
-        <v>736</v>
+        <v>754</v>
       </c>
       <c r="H169" t="n">
-        <v>5962401</v>
+        <v>844026814</v>
       </c>
       <c r="I169" t="n">
-        <v>1710.801</v>
+        <v>2535.262</v>
       </c>
       <c r="J169" t="n">
-        <v>7244</v>
+        <v>544070</v>
       </c>
       <c r="K169" t="n">
-        <v>2.079</v>
+        <v>1.634</v>
       </c>
       <c r="L169" t="n">
-        <v>11126</v>
+        <v>705786</v>
       </c>
       <c r="M169" t="n">
-        <v>3.192</v>
+        <v>2.12</v>
       </c>
       <c r="N169" t="n">
-        <v>0.1126</v>
+        <v>0.024</v>
       </c>
       <c r="O169" t="n">
-        <v>8.9</v>
+        <v>41.7</v>
       </c>
       <c r="P169" t="s">
-        <v>237</v>
+        <v>703</v>
       </c>
       <c r="Q169" t="s">
+        <v>702</v>
+      </c>
+      <c r="R169" t="s">
+        <v>704</v>
+      </c>
+      <c r="S169" t="s">
         <v>899</v>
-      </c>
-      <c r="R169" t="s">
-        <v>61</v>
-      </c>
-      <c r="S169" t="s">
-        <v>900</v>
       </c>
     </row>
     <row r="170">
       <c r="A170" t="s">
+        <v>900</v>
+      </c>
+      <c r="B170" t="s">
         <v>901</v>
       </c>
-      <c r="B170" t="s">
+      <c r="C170" s="1" t="n">
+        <v>44647</v>
+      </c>
+      <c r="D170" t="s">
         <v>902</v>
       </c>
-      <c r="C170" s="1" t="n">
-        <v>44619</v>
-      </c>
-      <c r="D170" t="s">
-        <v>903</v>
-      </c>
       <c r="E170" t="s">
-        <v>53</v>
+        <v>237</v>
       </c>
       <c r="F170"/>
       <c r="G170" t="n">
-        <v>2</v>
+        <v>736</v>
       </c>
       <c r="H170" t="n">
-        <v>11989</v>
+        <v>5962401</v>
       </c>
       <c r="I170" t="n">
-        <v>38.125</v>
-      </c>
-      <c r="J170"/>
-      <c r="K170"/>
+        <v>1710.801</v>
+      </c>
+      <c r="J170" t="n">
+        <v>7244</v>
+      </c>
+      <c r="K170" t="n">
+        <v>2.079</v>
+      </c>
       <c r="L170" t="n">
-        <v>76</v>
+        <v>11126</v>
       </c>
       <c r="M170" t="n">
-        <v>0.242</v>
+        <v>3.192</v>
       </c>
       <c r="N170" t="n">
-        <v>0.0132</v>
+        <v>0.1126</v>
       </c>
       <c r="O170" t="n">
-        <v>76</v>
+        <v>8.9</v>
       </c>
       <c r="P170" t="s">
-        <v>904</v>
+        <v>237</v>
       </c>
       <c r="Q170" t="s">
-        <v>905</v>
+        <v>902</v>
       </c>
       <c r="R170" t="s">
-        <v>311</v>
+        <v>61</v>
       </c>
       <c r="S170" t="s">
-        <v>906</v>
+        <v>903</v>
       </c>
     </row>
     <row r="171">
       <c r="A171" t="s">
-        <v>907</v>
+        <v>904</v>
       </c>
       <c r="B171" t="s">
-        <v>908</v>
+        <v>905</v>
       </c>
       <c r="C171" s="1" t="n">
-        <v>44648</v>
+        <v>44619</v>
       </c>
       <c r="D171" t="s">
-        <v>909</v>
+        <v>906</v>
       </c>
       <c r="E171" t="s">
-        <v>910</v>
+        <v>53</v>
       </c>
       <c r="F171"/>
       <c r="G171" t="n">
-        <v>152</v>
+        <v>2</v>
       </c>
       <c r="H171" t="n">
-        <v>84027988</v>
+        <v>11989</v>
       </c>
       <c r="I171" t="n">
-        <v>855.954</v>
+        <v>38.125</v>
       </c>
       <c r="J171"/>
       <c r="K171"/>
       <c r="L171" t="n">
-        <v>139911</v>
+        <v>76</v>
       </c>
       <c r="M171" t="n">
-        <v>1.425</v>
-      </c>
-      <c r="N171"/>
-      <c r="O171"/>
+        <v>0.242</v>
+      </c>
+      <c r="N171" t="n">
+        <v>0.0132</v>
+      </c>
+      <c r="O171" t="n">
+        <v>76</v>
+      </c>
       <c r="P171" t="s">
-        <v>911</v>
+        <v>907</v>
       </c>
       <c r="Q171" t="s">
-        <v>912</v>
+        <v>908</v>
       </c>
       <c r="R171" t="s">
-        <v>45</v>
+        <v>311</v>
       </c>
       <c r="S171" t="s">
-        <v>913</v>
+        <v>909</v>
       </c>
     </row>
     <row r="172">
       <c r="A172" t="s">
-        <v>914</v>
+        <v>910</v>
       </c>
       <c r="B172" t="s">
-        <v>915</v>
+        <v>911</v>
       </c>
       <c r="C172" s="1" t="n">
-        <v>44632</v>
+        <v>44648</v>
       </c>
       <c r="D172" t="s">
-        <v>21</v>
+        <v>912</v>
       </c>
       <c r="E172" t="s">
-        <v>22</v>
+        <v>913</v>
       </c>
       <c r="F172"/>
       <c r="G172" t="n">
-        <v>2</v>
+        <v>152</v>
       </c>
       <c r="H172" t="n">
-        <v>329592</v>
+        <v>84027988</v>
       </c>
       <c r="I172" t="n">
-        <v>10.81</v>
+        <v>855.954</v>
       </c>
       <c r="J172"/>
       <c r="K172"/>
       <c r="L172" t="n">
-        <v>0</v>
+        <v>139911</v>
       </c>
       <c r="M172" t="n">
-        <v>0</v>
+        <v>1.425</v>
       </c>
       <c r="N172"/>
       <c r="O172"/>
       <c r="P172" t="s">
-        <v>23</v>
+        <v>914</v>
       </c>
       <c r="Q172" t="s">
-        <v>24</v>
+        <v>915</v>
       </c>
       <c r="R172" t="s">
-        <v>25</v>
+        <v>45</v>
       </c>
       <c r="S172" t="s">
-        <v>26</v>
+        <v>916</v>
       </c>
     </row>
     <row r="173">
       <c r="A173" t="s">
-        <v>916</v>
+        <v>917</v>
       </c>
       <c r="B173" t="s">
-        <v>917</v>
+        <v>918</v>
       </c>
       <c r="C173" s="1" t="n">
-        <v>44646</v>
+        <v>44632</v>
       </c>
       <c r="D173" t="s">
-        <v>918</v>
+        <v>21</v>
       </c>
       <c r="E173" t="s">
-        <v>919</v>
+        <v>22</v>
       </c>
       <c r="F173"/>
       <c r="G173" t="n">
-        <v>710</v>
+        <v>2</v>
       </c>
       <c r="H173" t="n">
-        <v>3346905</v>
+        <v>329592</v>
       </c>
       <c r="I173" t="n">
-        <v>176.892</v>
-      </c>
-      <c r="J173" t="n">
-        <v>2364</v>
-      </c>
-      <c r="K173" t="n">
-        <v>0.125</v>
-      </c>
+        <v>10.81</v>
+      </c>
+      <c r="J173"/>
+      <c r="K173"/>
       <c r="L173" t="n">
-        <v>2674</v>
+        <v>0</v>
       </c>
       <c r="M173" t="n">
-        <v>0.141</v>
-      </c>
-      <c r="N173" t="n">
-        <v>0.0469</v>
-      </c>
-      <c r="O173" t="n">
-        <v>21.3</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="N173"/>
+      <c r="O173"/>
       <c r="P173" t="s">
-        <v>920</v>
+        <v>23</v>
       </c>
       <c r="Q173" t="s">
-        <v>918</v>
+        <v>24</v>
       </c>
       <c r="R173" t="s">
-        <v>61</v>
+        <v>25</v>
       </c>
       <c r="S173" t="s">
-        <v>921</v>
+        <v>26</v>
       </c>
     </row>
     <row r="174">
       <c r="A174" t="s">
+        <v>919</v>
+      </c>
+      <c r="B174" t="s">
+        <v>920</v>
+      </c>
+      <c r="C174" s="1" t="n">
+        <v>44646</v>
+      </c>
+      <c r="D174" t="s">
+        <v>921</v>
+      </c>
+      <c r="E174" t="s">
         <v>922</v>
-      </c>
-      <c r="B174" t="s">
-        <v>923</v>
-      </c>
-      <c r="C174" s="1" t="n">
-        <v>44648</v>
-      </c>
-      <c r="D174" t="s">
-        <v>35</v>
-      </c>
-      <c r="E174" t="s">
-        <v>36</v>
       </c>
       <c r="F174"/>
       <c r="G174" t="n">
-        <v>654</v>
+        <v>710</v>
       </c>
       <c r="H174" t="n">
-        <v>2176708</v>
+        <v>3346905</v>
       </c>
       <c r="I174" t="n">
-        <v>144.228</v>
-      </c>
-      <c r="J174"/>
-      <c r="K174"/>
+        <v>176.892</v>
+      </c>
+      <c r="J174" t="n">
+        <v>2364</v>
+      </c>
+      <c r="K174" t="n">
+        <v>0.125</v>
+      </c>
       <c r="L174" t="n">
-        <v>2747</v>
+        <v>2674</v>
       </c>
       <c r="M174" t="n">
-        <v>0.182</v>
-      </c>
-      <c r="N174"/>
-      <c r="O174"/>
+        <v>0.141</v>
+      </c>
+      <c r="N174" t="n">
+        <v>0.0469</v>
+      </c>
+      <c r="O174" t="n">
+        <v>21.3</v>
+      </c>
       <c r="P174" t="s">
-        <v>36</v>
+        <v>923</v>
       </c>
       <c r="Q174" t="s">
-        <v>37</v>
+        <v>921</v>
       </c>
       <c r="R174" t="s">
         <v>61</v>
       </c>
       <c r="S174" t="s">
         <v>924</v>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" t="s">
+        <v>925</v>
+      </c>
+      <c r="B175" t="s">
+        <v>926</v>
+      </c>
+      <c r="C175" s="1" t="n">
+        <v>44648</v>
+      </c>
+      <c r="D175" t="s">
+        <v>35</v>
+      </c>
+      <c r="E175" t="s">
+        <v>36</v>
+      </c>
+      <c r="F175"/>
+      <c r="G175" t="n">
+        <v>654</v>
+      </c>
+      <c r="H175" t="n">
+        <v>2176708</v>
+      </c>
+      <c r="I175" t="n">
+        <v>144.228</v>
+      </c>
+      <c r="J175"/>
+      <c r="K175"/>
+      <c r="L175" t="n">
+        <v>2747</v>
+      </c>
+      <c r="M175" t="n">
+        <v>0.182</v>
+      </c>
+      <c r="N175" t="n">
+        <v>0.0646</v>
+      </c>
+      <c r="O175" t="n">
+        <v>15.5</v>
+      </c>
+      <c r="P175" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q175" t="s">
+        <v>37</v>
+      </c>
+      <c r="R175" t="s">
+        <v>61</v>
+      </c>
+      <c r="S175" t="s">
+        <v>927</v>
       </c>
     </row>
   </sheetData>

</xml_diff>